<commit_message>
working default changed to KMIALL
</commit_message>
<xml_diff>
--- a/D-Advance_Technical_Analysis_QSE_STRONG_BUY.xlsx
+++ b/D-Advance_Technical_Analysis_QSE_STRONG_BUY.xlsx
@@ -1103,7 +1103,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B21" t="s">
         <v>37</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B23" t="s">
         <v>39</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B30" t="s">
         <v>46</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B39" t="s">
         <v>22</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B43" t="s">
         <v>26</v>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B44" t="s">
         <v>51</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B45" t="s">
         <v>27</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B46" t="s">
         <v>28</v>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B47" t="s">
         <v>29</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B48" t="s">
         <v>52</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B49" t="s">
         <v>53</v>
@@ -3791,7 +3791,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B50" t="s">
         <v>30</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -4071,7 +4071,7 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B55" t="s">
         <v>34</v>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B56" t="s">
         <v>35</v>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B57" t="s">
         <v>55</v>
@@ -4239,7 +4239,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B58" t="s">
         <v>36</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B59" t="s">
         <v>37</v>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B60" t="s">
         <v>56</v>
@@ -4407,7 +4407,7 @@
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B62" t="s">
         <v>39</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B63" t="s">
         <v>57</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B64" t="s">
         <v>40</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B65" t="s">
         <v>58</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B66" t="s">
         <v>41</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B67" t="s">
         <v>42</v>
@@ -4799,7 +4799,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B68" t="s">
         <v>59</v>
@@ -4855,7 +4855,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B69" t="s">
         <v>43</v>
@@ -4911,7 +4911,7 @@
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B70" t="s">
         <v>60</v>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B71" t="s">
         <v>61</v>
@@ -5023,7 +5023,7 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B72" t="s">
         <v>62</v>
@@ -5079,7 +5079,7 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B73" t="s">
         <v>63</v>
@@ -5135,7 +5135,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B74" t="s">
         <v>44</v>
@@ -5191,7 +5191,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B75" t="s">
         <v>45</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B76" t="s">
         <v>46</v>
@@ -5303,7 +5303,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B77" t="s">
         <v>64</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B78" t="s">
         <v>47</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B17" t="s">
         <v>52</v>
@@ -6692,7 +6692,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B26" t="s">
         <v>63</v>
@@ -7347,7 +7347,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2">
-        <v>45295.0834225</v>
+        <v>45295.08621759259</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -7403,7 +7403,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -7459,7 +7459,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -7515,7 +7515,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="2">
-        <v>45295.0862175947</v>
+        <v>45295.13199721622</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>

</xml_diff>